<commit_message>
2019 S2 & Tutorial 8
</commit_message>
<xml_diff>
--- a/LIRV/Textbook/LI&R Valuation S1 2020 M06 Table 6.16 - 6.17 Unit Linked 1pc entry fee.xlsx
+++ b/LIRV/Textbook/LI&R Valuation S1 2020 M06 Table 6.16 - 6.17 Unit Linked 1pc entry fee.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jizhu\Desktop\LIRV\Textbook\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jizhu\Documents\GitHub\my_file\LIRV\Textbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
@@ -149,7 +149,26 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Assume the profit is released at the start of the year.</t>
+Assume </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>all</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> the profits are released at the start of the year.</t>
         </r>
       </text>
     </comment>
@@ -667,9 +686,9 @@
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="0.00000"/>
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0"/>
-    <numFmt numFmtId="167" formatCode="#,##0.00;[Red]\(#,##0.00\)"/>
-    <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00;[Red]\(#,##0.00\)"/>
+    <numFmt numFmtId="167" formatCode="0.0%"/>
   </numFmts>
   <fonts count="24" x14ac:knownFonts="1">
     <font>
@@ -1233,13 +1252,13 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1259,16 +1278,16 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="8" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1290,72 +1309,99 @@
     <xf numFmtId="1" fontId="8" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="18" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="18" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1363,6 +1409,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1380,16 +1438,10 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1404,10 +1456,10 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1415,39 +1467,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="18" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="18" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="21" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="23" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3110,7 +3129,7 @@
       <pane xSplit="7" ySplit="5" topLeftCell="H6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="L28" sqref="L28"/>
+      <selection pane="bottomRight" activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -3159,7 +3178,7 @@
     </row>
     <row r="6" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="I6" s="80" t="s">
+      <c r="I6" s="60" t="s">
         <v>115</v>
       </c>
       <c r="J6"/>
@@ -3170,7 +3189,7 @@
         <v>117</v>
       </c>
       <c r="Q6" s="3"/>
-      <c r="R6" s="87">
+      <c r="R6" s="65">
         <f>N9/'Policyholder cash flows'!H6</f>
         <v>0.35829637242248791</v>
       </c>
@@ -3178,63 +3197,63 @@
         <v>118</v>
       </c>
       <c r="AF6" s="3"/>
-      <c r="AG6" s="87">
+      <c r="AG6" s="65">
         <f>AF9/'Policyholder cash flows'!H6</f>
         <v>0.25439561256186638</v>
       </c>
-      <c r="AH6" s="89" t="s">
+      <c r="AH6" s="67" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I7" s="81" t="s">
+      <c r="I7" s="74" t="s">
         <v>73</v>
       </c>
-      <c r="J7" s="68" t="s">
+      <c r="J7" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="K7" s="69"/>
-      <c r="L7" s="69"/>
-      <c r="M7" s="69"/>
-      <c r="N7" s="69"/>
-      <c r="P7" s="68" t="s">
+      <c r="K7" s="77"/>
+      <c r="L7" s="77"/>
+      <c r="M7" s="77"/>
+      <c r="N7" s="77"/>
+      <c r="P7" s="76" t="s">
         <v>50</v>
       </c>
-      <c r="Q7" s="69"/>
-      <c r="R7" s="69"/>
-      <c r="S7" s="69"/>
-      <c r="T7" s="69"/>
-      <c r="U7" s="69"/>
-      <c r="V7" s="69"/>
-      <c r="W7" s="69"/>
-      <c r="Y7" s="68" t="s">
+      <c r="Q7" s="77"/>
+      <c r="R7" s="77"/>
+      <c r="S7" s="77"/>
+      <c r="T7" s="77"/>
+      <c r="U7" s="77"/>
+      <c r="V7" s="77"/>
+      <c r="W7" s="77"/>
+      <c r="Y7" s="76" t="s">
         <v>58</v>
       </c>
-      <c r="Z7" s="69"/>
-      <c r="AA7" s="69"/>
-      <c r="AB7" s="69"/>
-      <c r="AC7" s="69"/>
-      <c r="AE7" s="90" t="s">
+      <c r="Z7" s="77"/>
+      <c r="AA7" s="77"/>
+      <c r="AB7" s="77"/>
+      <c r="AC7" s="77"/>
+      <c r="AE7" s="69" t="s">
         <v>96</v>
       </c>
-      <c r="AF7" s="91"/>
-      <c r="AG7" s="91"/>
-      <c r="AH7" s="91"/>
-      <c r="AI7" s="91"/>
-      <c r="AJ7" s="91"/>
-      <c r="AK7" s="91"/>
-      <c r="AL7" s="91"/>
+      <c r="AF7" s="70"/>
+      <c r="AG7" s="70"/>
+      <c r="AH7" s="70"/>
+      <c r="AI7" s="70"/>
+      <c r="AJ7" s="70"/>
+      <c r="AK7" s="70"/>
+      <c r="AL7" s="70"/>
     </row>
     <row r="8" spans="1:38" ht="54" x14ac:dyDescent="0.25">
-      <c r="B8" s="60" t="s">
+      <c r="B8" s="71" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="61"/>
-      <c r="D8" s="61"/>
-      <c r="E8" s="61"/>
-      <c r="F8" s="61"/>
-      <c r="G8" s="62"/>
-      <c r="I8" s="82"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="72"/>
+      <c r="G8" s="73"/>
+      <c r="I8" s="75"/>
       <c r="J8" s="22" t="s">
         <v>33</v>
       </c>
@@ -3337,7 +3356,7 @@
       <c r="I9" s="5">
         <v>0</v>
       </c>
-      <c r="J9" s="83">
+      <c r="J9" s="61">
         <f>NPV(Discount_rate,'Shareholder cash flows'!$D10:$D$20)*(1+Discount_rate)-D10
 +NPV(Discount_rate,'Shareholder cash flows'!$E10:$E$20)*(1+Discount_rate)-E10
 +NPV(Discount_rate,'Shareholder cash flows'!$F10:$F$20)
@@ -3349,11 +3368,11 @@
         <f>J9</f>
         <v>9318.3156039411988</v>
       </c>
-      <c r="M9" s="83">
+      <c r="M9" s="61">
         <f>C10-D10-E10+K9-L9</f>
         <v>281.68439605880121</v>
       </c>
-      <c r="N9" s="84">
+      <c r="N9" s="62">
         <f>NPV(Discount_rate,'Shareholder cash flows'!$M10:$M$20)+M9</f>
         <v>281.68439605879911</v>
       </c>
@@ -3374,14 +3393,14 @@
         <f>R9</f>
         <v>9599.9999999999982</v>
       </c>
-      <c r="U9" s="83">
+      <c r="U9" s="61">
         <f>C10-D10-E10+S9-T9</f>
         <v>0</v>
       </c>
       <c r="V9" s="24">
         <v>0</v>
       </c>
-      <c r="W9" s="84">
+      <c r="W9" s="62">
         <f>NPV(Discount_rate,'Shareholder cash flows'!$U10:$U$20)+U9</f>
         <v>281.68439605879502</v>
       </c>
@@ -3394,11 +3413,11 @@
         <f>Y9</f>
         <v>9900</v>
       </c>
-      <c r="AB9" s="85">
+      <c r="AB9" s="63">
         <f>C10-D10-E10+Z9-AA9</f>
         <v>-300</v>
       </c>
-      <c r="AC9" s="84">
+      <c r="AC9" s="62">
         <f>NPV(Discount_rate,AB10:AB20)+AB9</f>
         <v>281.68439605879678</v>
       </c>
@@ -3406,7 +3425,7 @@
         <f>Y9</f>
         <v>9900</v>
       </c>
-      <c r="AF9" s="86">
+      <c r="AF9" s="64">
         <f>Single_premium*(Initial_comm_rate-Entry_fee)</f>
         <v>199.99999999999997</v>
       </c>
@@ -3418,16 +3437,16 @@
         <f>AE9-AF9</f>
         <v>9700</v>
       </c>
-      <c r="AI9" s="84"/>
+      <c r="AI9" s="62"/>
       <c r="AJ9" s="24">
         <f>AH9</f>
         <v>9700</v>
       </c>
-      <c r="AK9" s="85">
+      <c r="AK9" s="63">
         <f>C10-D10-E10+AI9-AJ9</f>
         <v>-100</v>
       </c>
-      <c r="AL9" s="84">
+      <c r="AL9" s="62">
         <f>NPV(Discount_rate,AK10:AK20)+AK9</f>
         <v>281.68439605879701</v>
       </c>
@@ -3467,7 +3486,7 @@
 -NPV(Discount_rate,'Shareholder cash flows'!$C11:$C$20)*(1+Discount_rate)</f>
         <v>7808.3145401776728</v>
       </c>
-      <c r="K10" s="83">
+      <c r="K10" s="61">
         <f>J9*Investment_rate</f>
         <v>559.0989362364719</v>
       </c>
@@ -3475,11 +3494,11 @@
         <f>J10-J9</f>
         <v>-1510.001063763526</v>
       </c>
-      <c r="M10" s="83">
+      <c r="M10" s="61">
         <f>-F10+K10-L10</f>
         <v>0</v>
       </c>
-      <c r="N10" s="88">
+      <c r="N10" s="66">
         <f>M9*(1+Investment_rate)+M10</f>
         <v>298.58545982232931</v>
       </c>
@@ -3496,7 +3515,7 @@
         <f t="shared" si="0"/>
         <v>8053.6929886952603</v>
       </c>
-      <c r="S10" s="85">
+      <c r="S10" s="63">
         <f>(R9)*Investment_rate</f>
         <v>575.99999999999989</v>
       </c>
@@ -3504,7 +3523,7 @@
         <f>R10-R9</f>
         <v>-1546.3070113047379</v>
       </c>
-      <c r="U10" s="83">
+      <c r="U10" s="61">
         <f>-F10+S10-T10</f>
         <v>53.207011304738444</v>
       </c>
@@ -3516,7 +3535,7 @@
         <f>'Policyholder cash flows'!D7</f>
         <v>8276.4000000000015</v>
       </c>
-      <c r="Z10" s="83">
+      <c r="Z10" s="61">
         <f>Y9*Investment_rate</f>
         <v>594</v>
       </c>
@@ -3524,11 +3543,11 @@
         <f t="shared" ref="AA10:AA19" si="2">Y10-Y9</f>
         <v>-1623.5999999999985</v>
       </c>
-      <c r="AB10" s="85">
+      <c r="AB10" s="63">
         <f>-F10+Z10-AA10</f>
         <v>148.49999999999909</v>
       </c>
-      <c r="AC10" s="88">
+      <c r="AC10" s="66">
         <f>AB9*(1+Investment_rate)+AB10</f>
         <v>-169.50000000000091</v>
       </c>
@@ -3536,8 +3555,8 @@
         <f t="shared" ref="AE10:AE18" si="3">Y10</f>
         <v>8276.4000000000015</v>
       </c>
-      <c r="AF10" s="92">
-        <f>AF9*(1+Investment_rate)-AG9</f>
+      <c r="AF10" s="68">
+        <f t="shared" ref="AF10:AF19" si="4">AF9*(1+Investment_rate)-AG9</f>
         <v>174.22225153456282</v>
       </c>
       <c r="AG10" s="24">
@@ -3545,22 +3564,22 @@
         <v>31.582197717105469</v>
       </c>
       <c r="AH10" s="24">
-        <f t="shared" ref="AH10:AH19" si="4">AE10-AF10</f>
+        <f t="shared" ref="AH10:AH19" si="5">AE10-AF10</f>
         <v>8102.1777484654385</v>
       </c>
-      <c r="AI10" s="83">
+      <c r="AI10" s="61">
         <f>(AH9)*Investment_rate</f>
         <v>582</v>
       </c>
       <c r="AJ10" s="24">
-        <f t="shared" ref="AJ10:AJ19" si="5">AH10-AH9</f>
+        <f t="shared" ref="AJ10:AJ19" si="6">AH10-AH9</f>
         <v>-1597.8222515345615</v>
       </c>
-      <c r="AK10" s="85">
+      <c r="AK10" s="63">
         <f>-F10+AI10-AJ10</f>
         <v>110.72225153456202</v>
       </c>
-      <c r="AL10" s="88">
+      <c r="AL10" s="66">
         <f>AK9*(1+Investment_rate)+AK10</f>
         <v>4.7222515345620195</v>
       </c>
@@ -3585,12 +3604,12 @@
         <v>864.88380000000097</v>
       </c>
       <c r="G11" s="8">
-        <f t="shared" ref="G11:G19" si="6">C11-D11-E11-F11</f>
+        <f t="shared" ref="G11:G19" si="7">C11-D11-E11-F11</f>
         <v>-904.88380000000097</v>
       </c>
       <c r="H11" s="9"/>
       <c r="I11" s="5">
-        <f t="shared" ref="I11:I19" si="7">1+I10</f>
+        <f t="shared" ref="I11:I19" si="8">1+I10</f>
         <v>2</v>
       </c>
       <c r="J11" s="8">
@@ -3601,11 +3620,11 @@
         <v>7369.5296125883324</v>
       </c>
       <c r="K11" s="8">
-        <f>(J10+C11-D11-E11)*Investment_rate</f>
+        <f t="shared" ref="K11:K19" si="9">(J10+C11-D11-E11)*Investment_rate</f>
         <v>466.09887241066036</v>
       </c>
       <c r="L11" s="8">
-        <f t="shared" ref="L11:L19" si="8">J11-J10</f>
+        <f t="shared" ref="L11:L19" si="10">J11-J10</f>
         <v>-438.78492758934044</v>
       </c>
       <c r="M11" s="8">
@@ -3625,15 +3644,15 @@
         <v>7585.1497065662134</v>
       </c>
       <c r="S11" s="24">
-        <f t="shared" ref="S11:S19" si="9">(R10-E11-D11)*Investment_rate</f>
+        <f t="shared" ref="S11:S19" si="11">(R10-E11-D11)*Investment_rate</f>
         <v>480.8215793217156</v>
       </c>
       <c r="T11" s="24">
-        <f t="shared" ref="T11:T19" si="10">R11-R10</f>
+        <f t="shared" ref="T11:T19" si="12">R11-R10</f>
         <v>-468.54328212904693</v>
       </c>
       <c r="U11" s="24">
-        <f t="shared" ref="U11:U19" si="11">G11+S11-T11</f>
+        <f t="shared" ref="U11:U19" si="13">G11+S11-T11</f>
         <v>44.481061450761558</v>
       </c>
       <c r="V11" s="24">
@@ -3645,7 +3664,7 @@
         <v>7783.9542000000001</v>
       </c>
       <c r="Z11" s="23">
-        <f t="shared" ref="Z11:Z19" si="12">(Y10-D11-E11)*Investment_rate</f>
+        <f t="shared" ref="Z11:Z19" si="14">(Y10-D11-E11)*Investment_rate</f>
         <v>494.18400000000008</v>
       </c>
       <c r="AA11" s="24">
@@ -3653,7 +3672,7 @@
         <v>-492.44580000000133</v>
       </c>
       <c r="AB11" s="24">
-        <f t="shared" ref="AB11:AB19" si="13">G11+Z11-AA11</f>
+        <f t="shared" ref="AB11:AB19" si="15">G11+Z11-AA11</f>
         <v>81.746000000000436</v>
       </c>
       <c r="AC11"/>
@@ -3661,8 +3680,8 @@
         <f t="shared" si="3"/>
         <v>7783.9542000000001</v>
       </c>
-      <c r="AF11" s="92">
-        <f>AF10*(1+Investment_rate)-AG10</f>
+      <c r="AF11" s="68">
+        <f t="shared" si="4"/>
         <v>153.09338890953114</v>
       </c>
       <c r="AG11" s="24">
@@ -3670,15 +3689,15 @@
         <v>29.703056952937686</v>
       </c>
       <c r="AH11" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7630.8608110904688</v>
       </c>
       <c r="AI11" s="24">
-        <f>(AH10+C11-D11-E11)*Investment_rate</f>
+        <f t="shared" ref="AI11:AI19" si="16">(AH10+C11-D11-E11)*Investment_rate</f>
         <v>483.73066490792627</v>
       </c>
       <c r="AJ11" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-471.31693737496971</v>
       </c>
       <c r="AK11" s="24">
@@ -3688,7 +3707,7 @@
     </row>
     <row r="12" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" s="5">
-        <f t="shared" ref="B12:B19" si="14">1+B11</f>
+        <f t="shared" ref="B12:B19" si="17">1+B11</f>
         <v>3</v>
       </c>
       <c r="C12" s="8">
@@ -3706,12 +3725,12 @@
         <v>813.42321389999984</v>
       </c>
       <c r="G12" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-850.14321389999986</v>
       </c>
       <c r="H12"/>
       <c r="I12" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="J12" s="8">
@@ -3722,15 +3741,15 @@
         <v>6959.3549754436335</v>
       </c>
       <c r="K12" s="8">
-        <f>(J11+C12-D12-E12)*Investment_rate</f>
+        <f t="shared" si="9"/>
         <v>439.96857675529992</v>
       </c>
       <c r="L12" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-410.17463714469886</v>
       </c>
       <c r="M12" s="8">
-        <f t="shared" ref="M12:M19" si="15">G12+K12-L12</f>
+        <f t="shared" ref="M12:M19" si="18">G12+K12-L12</f>
         <v>-1.0800249583553523E-12</v>
       </c>
       <c r="P12" s="23">
@@ -3746,15 +3765,15 @@
         <v>7146.0778367657449</v>
       </c>
       <c r="S12" s="24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>452.90578239397274</v>
       </c>
       <c r="T12" s="24">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-439.07186980046845</v>
       </c>
       <c r="U12" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>41.834438294441327</v>
       </c>
       <c r="V12" s="24">
@@ -3766,7 +3785,7 @@
         <v>7320.808925100001</v>
       </c>
       <c r="Z12" s="23">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>464.83405199999999</v>
       </c>
       <c r="AA12" s="24">
@@ -3774,7 +3793,7 @@
         <v>-463.14527489999909</v>
       </c>
       <c r="AB12" s="24">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>77.836112999999216</v>
       </c>
       <c r="AC12"/>
@@ -3782,8 +3801,8 @@
         <f t="shared" si="3"/>
         <v>7320.808925100001</v>
       </c>
-      <c r="AF12" s="92">
-        <f>AF11*(1+Investment_rate)-AG11</f>
+      <c r="AF12" s="68">
+        <f t="shared" si="4"/>
         <v>132.57593529116534</v>
       </c>
       <c r="AG12" s="24">
@@ -3791,25 +3810,25 @@
         <v>27.9357250642379</v>
       </c>
       <c r="AH12" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7188.2329898088356</v>
       </c>
       <c r="AI12" s="24">
-        <f>(AH11+C12-D12-E12)*Investment_rate</f>
+        <f t="shared" si="16"/>
         <v>455.64844866542808</v>
       </c>
       <c r="AJ12" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-442.62782128163326</v>
       </c>
       <c r="AK12" s="24">
-        <f t="shared" ref="AK12:AK19" si="16">G12+AI12-AJ12</f>
+        <f t="shared" ref="AK12:AK19" si="19">G12+AI12-AJ12</f>
         <v>48.133056047061473</v>
       </c>
     </row>
     <row r="13" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="B13" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>4</v>
       </c>
       <c r="C13" s="8">
@@ -3827,12 +3846,12 @@
         <v>765.02453267294993</v>
       </c>
       <c r="G13" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-798.73349267294998</v>
       </c>
       <c r="H13"/>
       <c r="I13" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="J13" s="8">
@@ -3843,15 +3862,15 @@
         <v>6576.1602436973008</v>
       </c>
       <c r="K13" s="8">
-        <f>(J12+C13-D13-E13)*Investment_rate</f>
+        <f t="shared" si="9"/>
         <v>415.53876092661801</v>
       </c>
       <c r="L13" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-383.19473174633276</v>
       </c>
       <c r="M13" s="8">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>7.9580786405131221E-13</v>
       </c>
       <c r="P13" s="23">
@@ -3867,15 +3886,15 @@
         <v>6734.7411874828167</v>
       </c>
       <c r="S13" s="24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>426.74213260594468</v>
       </c>
       <c r="T13" s="24">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-411.33664928292819</v>
       </c>
       <c r="U13" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>39.34528921592289</v>
       </c>
       <c r="V13" s="24">
@@ -3887,7 +3906,7 @@
         <v>6885.2207940565504</v>
       </c>
       <c r="Z13" s="23">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>437.22599790600003</v>
       </c>
       <c r="AA13" s="24">
@@ -3895,7 +3914,7 @@
         <v>-435.58813104345063</v>
       </c>
       <c r="AB13" s="24">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>74.080636276500684</v>
       </c>
       <c r="AC13"/>
@@ -3903,8 +3922,8 @@
         <f t="shared" si="3"/>
         <v>6885.2207940565504</v>
       </c>
-      <c r="AF13" s="92">
-        <f>AF12*(1+Investment_rate)-AG12</f>
+      <c r="AF13" s="68">
+        <f t="shared" si="4"/>
         <v>112.59476634439737</v>
       </c>
       <c r="AG13" s="24">
@@ -3912,25 +3931,25 @@
         <v>26.273549422915739</v>
       </c>
       <c r="AH13" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6772.6260277121528</v>
       </c>
       <c r="AI13" s="24">
-        <f>(AH12+C13-D13-E13)*Investment_rate</f>
+        <f t="shared" si="16"/>
         <v>429.27144178853013</v>
       </c>
       <c r="AJ13" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-415.60696209668276</v>
       </c>
       <c r="AK13" s="24">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>46.144911212262912</v>
       </c>
     </row>
     <row r="14" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="B14" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="C14" s="8">
@@ -3948,12 +3967,12 @@
         <v>719.50557297891021</v>
       </c>
       <c r="G14" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-750.45039825891024</v>
       </c>
       <c r="H14"/>
       <c r="I14" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="J14" s="8">
@@ -3964,15 +3983,15 @@
         <v>6218.4227705434296</v>
       </c>
       <c r="K14" s="8">
-        <f>(J13+C14-D14-E14)*Investment_rate</f>
+        <f t="shared" si="9"/>
         <v>392.71292510503804</v>
       </c>
       <c r="L14" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-357.73747315387118</v>
       </c>
       <c r="M14" s="8">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>-1.0231815394945443E-12</v>
       </c>
       <c r="P14" s="23">
@@ -3988,15 +4007,15 @@
         <v>6349.5143264485014</v>
       </c>
       <c r="S14" s="24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>402.22778173216898</v>
       </c>
       <c r="T14" s="24">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-385.22686103431533</v>
       </c>
       <c r="U14" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>37.004244507574072</v>
       </c>
       <c r="V14" s="24">
@@ -4008,7 +4027,7 @@
         <v>6475.5501568101854</v>
       </c>
       <c r="Z14" s="23">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>411.25655812659301</v>
       </c>
       <c r="AA14" s="24">
@@ -4016,7 +4035,7 @@
         <v>-409.670637246365</v>
       </c>
       <c r="AB14" s="24">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>70.47679711404777</v>
       </c>
       <c r="AC14"/>
@@ -4024,8 +4043,8 @@
         <f t="shared" si="3"/>
         <v>6475.5501568101854</v>
       </c>
-      <c r="AF14" s="92">
-        <f>AF13*(1+Investment_rate)-AG13</f>
+      <c r="AF14" s="68">
+        <f t="shared" si="4"/>
         <v>93.076902902145477</v>
       </c>
       <c r="AG14" s="24">
@@ -4033,25 +4052,25 @@
         <v>24.710273232252256</v>
       </c>
       <c r="AH14" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6382.4732539080396</v>
       </c>
       <c r="AI14" s="24">
-        <f>(AH13+C14-D14-E14)*Investment_rate</f>
+        <f t="shared" si="16"/>
         <v>404.50087214592912</v>
       </c>
       <c r="AJ14" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-390.15277380411317</v>
       </c>
       <c r="AK14" s="24">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>44.203247691132049</v>
       </c>
     </row>
     <row r="15" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>6</v>
       </c>
       <c r="C15" s="8">
@@ -4069,12 +4088,12 @@
         <v>676.69499138666424</v>
       </c>
       <c r="G15" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-705.10234099370427</v>
       </c>
       <c r="H15"/>
       <c r="I15" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="J15" s="8">
@@ -4085,15 +4104,15 @@
         <v>5884.721354805909</v>
       </c>
       <c r="K15" s="8">
-        <f>(J14+C15-D15-E15)*Investment_rate</f>
+        <f t="shared" si="9"/>
         <v>371.40092525618337</v>
       </c>
       <c r="L15" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-333.70141573752062</v>
       </c>
       <c r="M15" s="8">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="P15" s="23">
@@ -4109,15 +4128,15 @@
         <v>5988.8759121059102</v>
       </c>
       <c r="S15" s="24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>379.26641861048768</v>
       </c>
       <c r="T15" s="24">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-360.6384143425912</v>
       </c>
       <c r="U15" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>34.802491959374606</v>
       </c>
       <c r="V15" s="24">
@@ -4129,7 +4148,7 @@
         <v>6090.2549224799805</v>
       </c>
       <c r="Z15" s="23">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>386.82856843218872</v>
       </c>
       <c r="AA15" s="24">
@@ -4137,7 +4156,7 @@
         <v>-385.29523433020495</v>
       </c>
       <c r="AB15" s="24">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>67.021461768689392</v>
       </c>
       <c r="AC15"/>
@@ -4145,8 +4164,8 @@
         <f t="shared" si="3"/>
         <v>6090.2549224799805</v>
       </c>
-      <c r="AF15" s="92">
-        <f>AF14*(1+Investment_rate)-AG14</f>
+      <c r="AF15" s="68">
+        <f t="shared" si="4"/>
         <v>73.951243844021946</v>
       </c>
       <c r="AG15" s="24">
@@ -4154,25 +4173,25 @@
         <v>23.24001197493325</v>
       </c>
       <c r="AH15" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6016.3036786359589</v>
       </c>
       <c r="AI15" s="24">
-        <f>(AH14+C15-D15-E15)*Investment_rate</f>
+        <f t="shared" si="16"/>
         <v>381.24395425806</v>
       </c>
       <c r="AJ15" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-366.16957527208069</v>
       </c>
       <c r="AK15" s="24">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>42.311188536436418</v>
       </c>
     </row>
     <row r="16" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>7</v>
       </c>
       <c r="C16" s="8">
@@ -4190,12 +4209,12 @@
         <v>636.4316393991586</v>
       </c>
       <c r="G16" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-662.50958633842129</v>
       </c>
       <c r="H16"/>
       <c r="I16" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="J16" s="8">
@@ -4206,15 +4225,15 @@
         <v>5573.7303729394871</v>
       </c>
       <c r="K16" s="8">
-        <f>(J15+C16-D16-E16)*Investment_rate</f>
+        <f t="shared" si="9"/>
         <v>351.51860447199874</v>
       </c>
       <c r="L16" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-310.99098186642186</v>
       </c>
       <c r="M16" s="8">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>-6.8212102632969618E-13</v>
       </c>
       <c r="P16" s="23">
@@ -4230,15 +4249,15 @@
         <v>5651.4024599896975</v>
       </c>
       <c r="S16" s="24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>357.76787790999884</v>
       </c>
       <c r="T16" s="24">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-337.47345211621268</v>
       </c>
       <c r="U16" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>32.731743687790242</v>
       </c>
       <c r="V16" s="24">
@@ -4250,7 +4269,7 @@
         <v>5727.8847545924218</v>
       </c>
       <c r="Z16" s="23">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>363.85061853244304</v>
       </c>
       <c r="AA16" s="24">
@@ -4258,7 +4277,7 @@
         <v>-362.37016788755864</v>
       </c>
       <c r="AB16" s="24">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>63.711200081580387</v>
       </c>
       <c r="AC16"/>
@@ -4266,8 +4285,8 @@
         <f t="shared" si="3"/>
         <v>5727.8847545924218</v>
       </c>
-      <c r="AF16" s="92">
-        <f>AF15*(1+Investment_rate)-AG15</f>
+      <c r="AF16" s="68">
+        <f t="shared" si="4"/>
         <v>55.148306499730012</v>
       </c>
       <c r="AG16" s="24">
@@ -4275,25 +4294,25 @@
         <v>21.857231262424722</v>
       </c>
       <c r="AH16" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5672.7364480926917</v>
       </c>
       <c r="AI16" s="24">
-        <f>(AH15+C16-D16-E16)*Investment_rate</f>
+        <f t="shared" si="16"/>
         <v>359.41354390180175</v>
       </c>
       <c r="AJ16" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-343.56723054326721</v>
       </c>
       <c r="AK16" s="24">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>40.471188106647674</v>
       </c>
     </row>
     <row r="17" spans="2:37" ht="15" x14ac:dyDescent="0.25">
       <c r="B17" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>8</v>
       </c>
       <c r="C17" s="8">
@@ -4311,12 +4330,12 @@
         <v>598.56395685490793</v>
       </c>
       <c r="G17" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-622.50351214515115</v>
       </c>
       <c r="H17"/>
       <c r="I17" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="J17" s="8">
@@ -4327,15 +4346,15 @@
         <v>5284.2143098532915</v>
       </c>
       <c r="K17" s="8">
-        <f>(J16+C17-D17-E17)*Investment_rate</f>
+        <f t="shared" si="9"/>
         <v>332.98744905895461</v>
       </c>
       <c r="L17" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-289.51606308619557</v>
       </c>
       <c r="M17" s="8">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>-9.6633812063373625E-13</v>
       </c>
       <c r="P17" s="23">
@@ -4351,15 +4370,15 @@
         <v>5335.7625171881464</v>
       </c>
       <c r="S17" s="24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>337.64777428196726</v>
       </c>
       <c r="T17" s="24">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-315.63994280155111</v>
       </c>
       <c r="U17" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>30.784204938367225</v>
       </c>
       <c r="V17" s="24">
@@ -4371,7 +4390,7 @@
         <v>5387.0756116941729</v>
       </c>
       <c r="Z17" s="23">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>342.23671195813068</v>
       </c>
       <c r="AA17" s="24">
@@ -4379,7 +4398,7 @@
         <v>-340.80914289824887</v>
       </c>
       <c r="AB17" s="24">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>60.5423427112284</v>
       </c>
       <c r="AC17"/>
@@ -4387,8 +4406,8 @@
         <f t="shared" si="3"/>
         <v>5387.0756116941729</v>
       </c>
-      <c r="AF17" s="92">
-        <f>AF16*(1+Investment_rate)-AG16</f>
+      <c r="AF17" s="68">
+        <f t="shared" si="4"/>
         <v>36.599973627289089</v>
       </c>
       <c r="AG17" s="24">
@@ -4396,25 +4415,25 @@
         <v>20.556726002310452</v>
       </c>
       <c r="AH17" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5350.4756380668841</v>
       </c>
       <c r="AI17" s="24">
-        <f>(AH16+C17-D17-E17)*Investment_rate</f>
+        <f t="shared" si="16"/>
         <v>338.92781356814692</v>
       </c>
       <c r="AJ17" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-322.26081002580759</v>
       </c>
       <c r="AK17" s="24">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>38.685111448803355</v>
       </c>
     </row>
     <row r="18" spans="2:37" ht="15" x14ac:dyDescent="0.25">
       <c r="B18" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>9</v>
       </c>
       <c r="C18" s="8">
@@ -4432,12 +4451,12 @@
         <v>562.94940142204098</v>
       </c>
       <c r="G18" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-584.92591317848417</v>
       </c>
       <c r="H18"/>
       <c r="I18" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="J18" s="8">
@@ -4448,15 +4467,15 @@
         <v>5015.0226645606181</v>
       </c>
       <c r="K18" s="8">
-        <f>(J17+C18-D18-E18)*Investment_rate</f>
+        <f t="shared" si="9"/>
         <v>315.73426788581088</v>
       </c>
       <c r="L18" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-269.19164529267346</v>
       </c>
       <c r="M18" s="8">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="P18" s="23">
@@ -4472,15 +4491,15 @@
         <v>5040.7112195910286</v>
       </c>
       <c r="S18" s="24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>318.82716032590218</v>
       </c>
       <c r="T18" s="24">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-295.05129759711781</v>
       </c>
       <c r="U18" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>28.952544744535828</v>
       </c>
       <c r="V18" s="24">
@@ -4492,7 +4511,7 @@
         <v>5066.5446127983696</v>
       </c>
       <c r="Z18" s="23">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>321.90594599626377</v>
       </c>
       <c r="AA18" s="24">
@@ -4500,7 +4519,7 @@
         <v>-320.53099889580335</v>
       </c>
       <c r="AB18" s="24">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>57.511031713582952</v>
       </c>
       <c r="AC18"/>
@@ -4508,8 +4527,8 @@
         <f t="shared" si="3"/>
         <v>5066.5446127983696</v>
       </c>
-      <c r="AF18" s="92">
-        <f>AF17*(1+Investment_rate)-AG17</f>
+      <c r="AF18" s="68">
+        <f t="shared" si="4"/>
         <v>18.239246042615985</v>
       </c>
       <c r="AG18" s="24">
@@ -4517,15 +4536,15 @@
         <v>19.333600805172978</v>
       </c>
       <c r="AH18" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5048.3053667557533</v>
       </c>
       <c r="AI18" s="24">
-        <f>(AH17+C18-D18-E18)*Investment_rate</f>
+        <f t="shared" si="16"/>
         <v>319.70994757862644</v>
       </c>
       <c r="AJ18" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-302.17027131113082</v>
       </c>
       <c r="AK18" s="24">
@@ -4535,7 +4554,7 @@
     </row>
     <row r="19" spans="2:37" ht="15" x14ac:dyDescent="0.25">
       <c r="B19" s="5">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>10</v>
       </c>
       <c r="C19" s="8">
@@ -4553,12 +4572,12 @@
         <v>5294.5391203742956</v>
       </c>
       <c r="G19" s="8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-5314.7135581667108</v>
       </c>
       <c r="H19"/>
       <c r="I19" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="J19" s="8">
@@ -4569,15 +4588,15 @@
         <v>0</v>
       </c>
       <c r="K19" s="8">
-        <f>(J18+C19-D19-E19)*Investment_rate</f>
+        <f t="shared" si="9"/>
         <v>299.69089360609217</v>
       </c>
       <c r="L19" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>-5015.0226645606181</v>
       </c>
       <c r="M19" s="8">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="P19" s="23">
@@ -4593,15 +4612,15 @@
         <v>0</v>
       </c>
       <c r="S19" s="24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>301.2322069079168</v>
       </c>
       <c r="T19" s="24">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-5040.7112195910286</v>
       </c>
       <c r="U19" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>27.229868332234219</v>
       </c>
       <c r="V19" s="24">
@@ -4610,7 +4629,7 @@
       </c>
       <c r="Y19" s="23"/>
       <c r="Z19" s="23">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>302.78221050035728</v>
       </c>
       <c r="AA19" s="24">
@@ -4618,13 +4637,13 @@
         <v>-5066.5446127983696</v>
       </c>
       <c r="AB19" s="24">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>54.61326513201584</v>
       </c>
       <c r="AC19"/>
       <c r="AE19" s="23"/>
-      <c r="AF19" s="92">
-        <f>AF18*(1+Investment_rate)-AG18</f>
+      <c r="AF19" s="68">
+        <f t="shared" si="4"/>
         <v>-3.1974423109204508E-14</v>
       </c>
       <c r="AG19" s="24">
@@ -4632,19 +4651,19 @@
         <v>0</v>
       </c>
       <c r="AH19" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.1974423109204508E-14</v>
       </c>
       <c r="AI19" s="24">
-        <f>(AH18+C19-D19-E19)*Investment_rate</f>
+        <f t="shared" si="16"/>
         <v>301.68785573780031</v>
       </c>
       <c r="AJ19" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-5048.3053667557533</v>
       </c>
       <c r="AK19" s="24">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>35.279664326842976</v>
       </c>
     </row>
@@ -5163,17 +5182,17 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="71" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
-      <c r="H4" s="61"/>
-      <c r="I4" s="61"/>
-      <c r="J4" s="62"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="72"/>
+      <c r="E4" s="72"/>
+      <c r="F4" s="72"/>
+      <c r="G4" s="72"/>
+      <c r="H4" s="72"/>
+      <c r="I4" s="72"/>
+      <c r="J4" s="73"/>
     </row>
     <row r="5" spans="1:10" ht="40.5" x14ac:dyDescent="0.25">
       <c r="B5" s="57" t="s">
@@ -5592,8 +5611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K86"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="G71" sqref="G71"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -5625,18 +5644,18 @@
       <c r="E3" s="20"/>
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="63" t="s">
+      <c r="A5" s="78" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="64" t="s">
+      <c r="B5" s="79" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="66"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="81"/>
     </row>
     <row r="6" spans="1:10" ht="27" x14ac:dyDescent="0.25">
-      <c r="A6" s="67"/>
+      <c r="A6" s="82"/>
       <c r="B6" s="22" t="s">
         <v>33</v>
       </c>
@@ -5942,22 +5961,22 @@
       </c>
     </row>
     <row r="27" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="63" t="s">
+      <c r="A27" s="78" t="s">
         <v>73</v>
       </c>
-      <c r="B27" s="68" t="s">
+      <c r="B27" s="76" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="69"/>
-      <c r="D27" s="69"/>
-      <c r="E27" s="69"/>
-      <c r="F27" s="69"/>
-      <c r="G27" s="69"/>
-      <c r="H27" s="69"/>
+      <c r="C27" s="77"/>
+      <c r="D27" s="77"/>
+      <c r="E27" s="77"/>
+      <c r="F27" s="77"/>
+      <c r="G27" s="77"/>
+      <c r="H27" s="77"/>
       <c r="I27"/>
     </row>
     <row r="28" spans="1:11" ht="40.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="67"/>
+      <c r="A28" s="82"/>
       <c r="B28" s="22" t="s">
         <v>53</v>
       </c>
@@ -6408,21 +6427,21 @@
       <c r="H52"/>
     </row>
     <row r="53" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A53" s="63" t="s">
+      <c r="A53" s="78" t="s">
         <v>73</v>
       </c>
-      <c r="B53" s="64" t="s">
+      <c r="B53" s="79" t="s">
         <v>58</v>
       </c>
-      <c r="C53" s="65"/>
-      <c r="D53" s="65"/>
-      <c r="E53" s="66"/>
+      <c r="C53" s="80"/>
+      <c r="D53" s="80"/>
+      <c r="E53" s="81"/>
       <c r="F53"/>
       <c r="G53"/>
       <c r="H53"/>
     </row>
     <row r="54" spans="1:8" ht="27" x14ac:dyDescent="0.25">
-      <c r="A54" s="67"/>
+      <c r="A54" s="82"/>
       <c r="B54" s="22" t="s">
         <v>33</v>
       </c>
@@ -6791,21 +6810,21 @@
       <c r="H72"/>
     </row>
     <row r="73" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A73" s="63" t="s">
+      <c r="A73" s="78" t="s">
         <v>73</v>
       </c>
-      <c r="B73" s="64" t="s">
+      <c r="B73" s="79" t="s">
         <v>96</v>
       </c>
-      <c r="C73" s="65"/>
-      <c r="D73" s="65"/>
-      <c r="E73" s="66"/>
+      <c r="C73" s="80"/>
+      <c r="D73" s="80"/>
+      <c r="E73" s="81"/>
       <c r="F73"/>
       <c r="G73"/>
       <c r="H73"/>
     </row>
     <row r="74" spans="1:9" ht="54" x14ac:dyDescent="0.25">
-      <c r="A74" s="63"/>
+      <c r="A74" s="78"/>
       <c r="B74" s="53" t="s">
         <v>92</v>
       </c>
@@ -7239,36 +7258,36 @@
       <c r="B2" s="12"/>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="78" t="s">
+      <c r="A3" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="91" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="72" t="s">
+      <c r="C3" s="85" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="70" t="s">
+      <c r="D3" s="89" t="s">
         <v>82</v>
       </c>
-      <c r="E3" s="70" t="s">
+      <c r="E3" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="76" t="s">
+      <c r="F3" s="83" t="s">
         <v>83</v>
       </c>
-      <c r="G3" s="72" t="s">
+      <c r="G3" s="85" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="79"/>
-      <c r="B4" s="79"/>
-      <c r="C4" s="73"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="77"/>
-      <c r="G4" s="73"/>
+      <c r="A4" s="92"/>
+      <c r="B4" s="92"/>
+      <c r="C4" s="86"/>
+      <c r="D4" s="90"/>
+      <c r="E4" s="90"/>
+      <c r="F4" s="84"/>
+      <c r="G4" s="86"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="30">
@@ -7585,50 +7604,50 @@
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="72" t="s">
+      <c r="A24" s="85" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="74" t="s">
+      <c r="B24" s="87" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="70" t="s">
+      <c r="C24" s="89" t="s">
         <v>31</v>
       </c>
-      <c r="D24" s="70" t="s">
+      <c r="D24" s="89" t="s">
         <v>34</v>
       </c>
-      <c r="E24" s="70" t="s">
+      <c r="E24" s="89" t="s">
         <v>25</v>
       </c>
-      <c r="H24" s="72" t="s">
+      <c r="H24" s="85" t="s">
         <v>14</v>
       </c>
-      <c r="I24" s="74" t="s">
+      <c r="I24" s="87" t="s">
         <v>33</v>
       </c>
-      <c r="J24" s="70" t="s">
+      <c r="J24" s="89" t="s">
         <v>31</v>
       </c>
-      <c r="K24" s="70" t="s">
+      <c r="K24" s="89" t="s">
         <v>34</v>
       </c>
-      <c r="L24" s="70" t="s">
+      <c r="L24" s="89" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="73"/>
-      <c r="B25" s="75"/>
-      <c r="C25" s="71"/>
-      <c r="D25" s="71"/>
-      <c r="E25" s="71" t="s">
+      <c r="A25" s="86"/>
+      <c r="B25" s="88"/>
+      <c r="C25" s="90"/>
+      <c r="D25" s="90"/>
+      <c r="E25" s="90" t="s">
         <v>25</v>
       </c>
-      <c r="H25" s="73"/>
-      <c r="I25" s="75"/>
-      <c r="J25" s="71"/>
-      <c r="K25" s="71"/>
-      <c r="L25" s="71" t="s">
+      <c r="H25" s="86"/>
+      <c r="I25" s="88"/>
+      <c r="J25" s="90"/>
+      <c r="K25" s="90"/>
+      <c r="L25" s="90" t="s">
         <v>25</v>
       </c>
     </row>
@@ -8098,50 +8117,50 @@
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="72" t="s">
+      <c r="A40" s="85" t="s">
         <v>14</v>
       </c>
-      <c r="B40" s="74" t="s">
+      <c r="B40" s="87" t="s">
         <v>33</v>
       </c>
-      <c r="C40" s="70" t="s">
+      <c r="C40" s="89" t="s">
         <v>31</v>
       </c>
-      <c r="D40" s="70" t="s">
+      <c r="D40" s="89" t="s">
         <v>34</v>
       </c>
-      <c r="E40" s="70" t="s">
+      <c r="E40" s="89" t="s">
         <v>25</v>
       </c>
-      <c r="H40" s="72" t="s">
+      <c r="H40" s="85" t="s">
         <v>14</v>
       </c>
-      <c r="I40" s="74" t="s">
+      <c r="I40" s="87" t="s">
         <v>33</v>
       </c>
-      <c r="J40" s="70" t="s">
+      <c r="J40" s="89" t="s">
         <v>31</v>
       </c>
-      <c r="K40" s="70" t="s">
+      <c r="K40" s="89" t="s">
         <v>34</v>
       </c>
-      <c r="L40" s="70" t="s">
+      <c r="L40" s="89" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" s="73"/>
-      <c r="B41" s="75"/>
-      <c r="C41" s="71"/>
-      <c r="D41" s="71"/>
-      <c r="E41" s="71" t="s">
+      <c r="A41" s="86"/>
+      <c r="B41" s="88"/>
+      <c r="C41" s="90"/>
+      <c r="D41" s="90"/>
+      <c r="E41" s="90" t="s">
         <v>25</v>
       </c>
-      <c r="H41" s="73"/>
-      <c r="I41" s="75"/>
-      <c r="J41" s="71"/>
-      <c r="K41" s="71"/>
-      <c r="L41" s="71" t="s">
+      <c r="H41" s="86"/>
+      <c r="I41" s="88"/>
+      <c r="J41" s="90"/>
+      <c r="K41" s="90"/>
+      <c r="L41" s="90" t="s">
         <v>25</v>
       </c>
     </row>
@@ -8606,17 +8625,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
     <mergeCell ref="L24:L25"/>
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="B40:B41"/>
@@ -8633,6 +8641,17 @@
     <mergeCell ref="I24:I25"/>
     <mergeCell ref="J24:J25"/>
     <mergeCell ref="K24:K25"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>